<commit_message>
added concentrationFlag and EML evaluated
</commit_message>
<xml_diff>
--- a/level1b_edi.xlsx
+++ b/level1b_edi.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="65">
   <si>
     <t>attributeName</t>
   </si>
@@ -184,9 +184,6 @@
   </si>
   <si>
     <t>categorical</t>
-  </si>
-  <si>
-    <t>attribute</t>
   </si>
   <si>
     <t>code</t>
@@ -546,7 +543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -582,10 +579,10 @@
     </row>
     <row r="2" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -903,21 +900,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -925,10 +920,10 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -936,10 +931,10 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
         <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -947,10 +942,10 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
         <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -958,10 +953,10 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" t="s">
         <v>62</v>
-      </c>
-      <c r="C5" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>